<commit_message>
🚑 ✨ Add support for loading environment variables from .env file; enhance repository fetching with pagination and export to CSV/Excel
</commit_message>
<xml_diff>
--- a/missing_fields.xlsx
+++ b/missing_fields.xlsx
@@ -2861,7 +2861,7 @@
       </c>
       <c r="BC7" t="inlineStr"/>
       <c r="BD7" t="n">
-        <v>76</v>
+        <v>5005</v>
       </c>
       <c r="BE7" t="n">
         <v>0</v>
@@ -6712,7 +6712,7 @@
       </c>
       <c r="BC18" t="inlineStr"/>
       <c r="BD18" t="n">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="BE18" t="n">
         <v>0</v>
@@ -9145,12 +9145,12 @@
       </c>
       <c r="AW25" t="inlineStr">
         <is>
-          <t>2016-01-30T07:08:22Z</t>
+          <t>2025-01-01T05:32:11Z</t>
         </is>
       </c>
       <c r="AX25" t="inlineStr">
         <is>
-          <t>2014-05-18T11:11:19Z</t>
+          <t>2025-01-01T05:32:08Z</t>
         </is>
       </c>
       <c r="AY25" t="inlineStr">
@@ -9175,7 +9175,7 @@
       </c>
       <c r="BC25" t="inlineStr"/>
       <c r="BD25" t="n">
-        <v>419</v>
+        <v>74</v>
       </c>
       <c r="BE25" t="n">
         <v>0</v>

</xml_diff>